<commit_message>
Cambios previos a revisión final
</commit_message>
<xml_diff>
--- a/Listado Indicadores/Listado de indicadores a trabajar.xlsx
+++ b/Listado Indicadores/Listado de indicadores a trabajar.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inegobgt-my.sharepoint.com/personal/pgalvez_ine_gob_gt/Documents/Documentos/Proyectos/Compendio estadístico de género/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inegobgt-my.sharepoint.com/personal/pgalvez_ine_gob_gt/Documents/Documentos/GitHub/CompendioGenero2023/Listado Indicadores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="271" documentId="8_{33C4EBF3-B6E3-430A-80A9-911051E32003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{892A6980-E861-4EF2-98BC-458DA05FD67A}"/>
+  <xr:revisionPtr revIDLastSave="421" documentId="8_{33C4EBF3-B6E3-430A-80A9-911051E32003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D225325-2E87-49B9-A059-D9A04F5B6D22}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3D4A4D73-1AC6-4F09-9897-696579B6A714}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Cap 1." sheetId="2" r:id="rId2"/>
+    <sheet name="Listado indicadores" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$92</definedName>
+    <definedName name="_Hlk130380442" localSheetId="1">'Listado indicadores'!$C$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="262">
   <si>
     <t>Distribución de la población total por sexo según grupo de edad</t>
   </si>
@@ -392,14 +393,455 @@
     <t>Se sugiere cambiar el término vivienda por hogar para mayor claridad y continuidad con el compendio 2021</t>
   </si>
   <si>
-    <t>Indicadores que faltan</t>
-  </si>
-  <si>
-    <t>Compendio(s) en el que estaba</t>
-  </si>
-  <si>
-    <r>
-      <t>Tasa global de fecundidad por área</t>
+    <t>Agregada</t>
+  </si>
+  <si>
+    <t>sí</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>Se sugiera cambio de nombre a: Porcentaje de mujeres entre 15 y 49 años que han usado algún método de planificación familiar, según tipo de método. Fuente de 2008 es APROFAM, 2014 es ENCOVI, de 2013 ENSMI</t>
+  </si>
+  <si>
+    <t>Combinado con Tasa de alfabetismo por sexo</t>
+  </si>
+  <si>
+    <t>Combinado con Tasa global de alfabetismo</t>
+  </si>
+  <si>
+    <t>Combinado con Nivel educativo de la población de 15 años o más por sexo</t>
+  </si>
+  <si>
+    <t>Combinado con Población por sexo, según nivel de escolaridad</t>
+  </si>
+  <si>
+    <t>Cambiar USAC por tipo de universidad (pública o privada)</t>
+  </si>
+  <si>
+    <t>Agregar matriculación por sexo, campo de estudio en ambos tipos (pública o privadas) (En base a compendio 2014)</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Ver desagregación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se combinó con Salarios o ingresos promedio, desagregado por sexo y pueblo. </t>
+  </si>
+  <si>
+    <t>Se combinó con Diferencia salarial por área geográfica y sexo según rama de actividad económica.</t>
+  </si>
+  <si>
+    <t>Compara 2018 y 2022</t>
+  </si>
+  <si>
+    <t>Usar la más desagregada Población económicamente activa por sexo, pueblo de pertenencia y grupos de edad</t>
+  </si>
+  <si>
+    <t>Duplicada</t>
+  </si>
+  <si>
+    <t>Usar las otras dos de la PEA</t>
+  </si>
+  <si>
+    <t>Agregar desagregación de dominio de estudio</t>
+  </si>
+  <si>
+    <t>Usar Tasa de desempleo en la población de 15 años o más por sexo</t>
+  </si>
+  <si>
+    <t>% de denuncias de Violencia y intrafamiliar por sexo, según tipo de agresión sufrida</t>
+  </si>
+  <si>
+    <t>% de denuncias de Violencia y intrafamiliar por sexo, según grupos quinquenales de edad</t>
+  </si>
+  <si>
+    <t>Ya no se utiliza el grupo étnico</t>
+  </si>
+  <si>
+    <t>Agregar desagregación por sexo</t>
+  </si>
+  <si>
+    <t>Distribución porcentual de víctimas de Violencia según sexo y crímen intrafamiliar</t>
+  </si>
+  <si>
+    <t>Tasa promedio de denuncia por los delitos contemplado en la Ley Contra el Femicidio y Otras Formas de Violencia y crímen Contra a la Mujer, por departamento de registro</t>
+  </si>
+  <si>
+    <t>Desagregar por sexo</t>
+  </si>
+  <si>
+    <t>Usar la más desagregada Muertes violentas por sexo, según causa de muerte y grupos de edad</t>
+  </si>
+  <si>
+    <t>Participación porcentual en los Consejos de Desarrollo por sexo, según cargo</t>
+  </si>
+  <si>
+    <t>Discapacidad por sexo, según Pueblos</t>
+  </si>
+  <si>
+    <t>ENEI 2022</t>
+  </si>
+  <si>
+    <t>Se agrego en base a sugerenica Aurora</t>
+  </si>
+  <si>
+    <t>Jefatura de hogar por sexo según tipo de vivienda</t>
+  </si>
+  <si>
+    <t>Sugerenica Aurora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se sugirió poner mapa por sexo </t>
+  </si>
+  <si>
+    <t>Número de casos de mujeres embarazadas entre 15 y 49 años por Pueblos</t>
+  </si>
+  <si>
+    <t>Se sugirió el cambio: Nacimientos según grupos quinquenales de edad de la madre</t>
+  </si>
+  <si>
+    <t>Población entre 15 y 49 años que han usado algún método de planificación familiar por sexo</t>
+  </si>
+  <si>
+    <t>Paula sugirió</t>
+  </si>
+  <si>
+    <t>Tasa de mortalidad materna por causa de muerte</t>
+  </si>
+  <si>
+    <t>INACIF</t>
+  </si>
+  <si>
+    <t>Evelin sugirio</t>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <color rgb="FF2F5496"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF2F5496"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Población y demografía</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <color rgb="FF2F5496"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF2F5496"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Salud</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <color rgb="FF2F5496"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF2F5496"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Educación</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <color rgb="FF2F5496"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF2F5496"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Economía</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <color rgb="FF2F5496"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF2F5496"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Violencia</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <color rgb="FF2F5496"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF2F5496"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Participación sociopolítica</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Solo 2022.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel educativos es igual a nivel educativo completado</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PREGUNTARLE A HUGO!!!!!!!!!!!!!!!!!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Solo año 2022.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Indicadores en base a Compendio 2014. Solo año 2022.</t>
+    </r>
+  </si>
+  <si>
+    <t> Ver con Hugo la definición de la ficha técnica. Probablemente aquí: http://pnd.gt/Home/goals?code=ODS5</t>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Compendio 2007.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>El sector económico se desagrega en formal o informal.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Este rango de edad es el de la ENEI (que es el mismo del tablero). Va de 15 a 24 años y 25+.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Seguimiento a tablero en conmemoración del Día Internacional de la Mujer. Solo año 2022.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sugerencia Aurora.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Seguimiento a tablero en conmemoración del Día International de la Mujer.</t>
+    </r>
+  </si>
+  <si>
+    <t>Población por sexo, según grupo de edad simple</t>
+  </si>
+  <si>
+    <t>Población por sexo, según dominio de estudio</t>
+  </si>
+  <si>
+    <t>Población por sexo, según Pueblos</t>
+  </si>
+  <si>
+    <r>
+      <t>Población por sexo, según tipo de hogar</t>
     </r>
     <r>
       <rPr>
@@ -413,113 +855,1164 @@
     </r>
   </si>
   <si>
-    <t>Matrimonios por sexo, según pertenencia étnica</t>
-  </si>
-  <si>
-    <t>Matrimonios por sexo, según grupo de edad</t>
-  </si>
-  <si>
-    <t>Divorcios por sexo, según grupos de edad al añao de la sentencia</t>
-  </si>
-  <si>
-    <t>Tasa específica de fecundidad juvenil -TFJ- (edades de 13 a 19 años) de 2002 a 2011</t>
-  </si>
-  <si>
-    <t>Porcentaje de participación en la jefatura de hogar por sexo y pueblo de pertenencia según tipo de hogar</t>
-  </si>
-  <si>
-    <t>Agregada</t>
-  </si>
-  <si>
-    <t>sí</t>
-  </si>
-  <si>
-    <t>Sí</t>
-  </si>
-  <si>
-    <t>Se sugiera cambio de nombre a: Porcentaje de mujeres entre 15 y 49 años que han usado algún método de planificación familiar, según tipo de método. Fuente de 2008 es APROFAM, 2014 es ENCOVI, de 2013 ENSMI</t>
-  </si>
-  <si>
-    <t>Combinado con Tasa de alfabetismo por sexo</t>
-  </si>
-  <si>
-    <t>Combinado con Tasa global de alfabetismo</t>
-  </si>
-  <si>
-    <t>Combinado con Nivel educativo de la población de 15 años o más por sexo</t>
-  </si>
-  <si>
-    <t>Combinado con Población por sexo, según nivel de escolaridad</t>
-  </si>
-  <si>
-    <t>Cambiar USAC por tipo de universidad (pública o privada)</t>
-  </si>
-  <si>
-    <t>Agregar matriculación por sexo, campo de estudio en ambos tipos (pública o privadas) (En base a compendio 2014)</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Ver desagregación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se combinó con Salarios o ingresos promedio, desagregado por sexo y pueblo. </t>
-  </si>
-  <si>
-    <t>Se combinó con Diferencia salarial por área geográfica y sexo según rama de actividad económica.</t>
-  </si>
-  <si>
-    <t>Compara 2018 y 2022</t>
-  </si>
-  <si>
-    <t>Usar la más desagregada Población económicamente activa por sexo, pueblo de pertenencia y grupos de edad</t>
-  </si>
-  <si>
-    <t>Duplicada</t>
-  </si>
-  <si>
-    <t>Usar las otras dos de la PEA</t>
-  </si>
-  <si>
-    <t>Agregar desagregación de dominio de estudio</t>
-  </si>
-  <si>
-    <t>Usar Tasa de desempleo en la población de 15 años o más por sexo</t>
-  </si>
-  <si>
-    <t>% de denuncias de Violencia y intrafamiliar por sexo, según tipo de agresión sufrida</t>
-  </si>
-  <si>
-    <t>% de denuncias de Violencia y intrafamiliar por sexo, según grupos quinquenales de edad</t>
-  </si>
-  <si>
-    <t>Ya no se utiliza el grupo étnico</t>
-  </si>
-  <si>
-    <t>Agregar desagregación por sexo</t>
-  </si>
-  <si>
-    <t>Distribución porcentual de víctimas de Violencia según sexo y crímen intrafamiliar</t>
-  </si>
-  <si>
-    <t>Tasa promedio de denuncia por los delitos contemplado en la Ley Contra el Femicidio y Otras Formas de Violencia y crímen Contra a la Mujer, por departamento de registro</t>
-  </si>
-  <si>
-    <t>Desagregar por sexo</t>
-  </si>
-  <si>
-    <t>Usar la más desagregada Muertes violentas por sexo, según causa de muerte y grupos de edad</t>
-  </si>
-  <si>
-    <t>Participación porcentual en los Consejos de Desarrollo por sexo, según cargo</t>
+    <r>
+      <t>Población por sexo, según tipo de vivienda</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Mapa departamental por sexo, según departamento</t>
+  </si>
+  <si>
+    <t>Mapa municipal por sexo, según municipio</t>
+  </si>
+  <si>
+    <r>
+      <t>Esperanza de vida al nacer por sexo, según grupos de edad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tasa global de fecundidad (mujeres 15 a 49 años) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(serie histórica de 2018 a 2022)</t>
+    </r>
+  </si>
+  <si>
+    <t>Tasa de fecundidad juvenil según edades simples (13 -19 años)</t>
+  </si>
+  <si>
+    <t>Jefatura de hogar por sexo, según tipo de hogar</t>
+  </si>
+  <si>
+    <t>Acceso a servicios básicos por sexo de jefatura de hogar</t>
+  </si>
+  <si>
+    <t>Jefatura de hogar por sexo, según departamento</t>
+  </si>
+  <si>
+    <r>
+      <t>Jefatura de hogar por sexo, según estado civil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Mujeres jefas de hogar por número de hijas/hijos</t>
+  </si>
+  <si>
+    <r>
+      <t>Número de casos de mujeres embarazadas entre 15 y 49 años por Pueblo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(serie histórica de 2018 a 2022)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Población entre 15 y 49 años que han usado algún método de planificación familiar por tipo de método</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Nacimientos por edad de la madre, según grupos de edad</t>
+  </si>
+  <si>
+    <r>
+      <t>Porcentaje de partos atendidos, por tipo de asistencia</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(serie histórica de 2018 a 2022)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Discapacidad por </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sexo, según grupos de edad</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Discapacidad por </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sexo, según Pueblos</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Porcentaje de personas notificadas con VIH/SIDA, por sexo, según grupos de edad </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(serie histórica de 2018 a 2023)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Número de casos de mujeres seropositivas embarazadas entre 15 y 49 años por Pueblo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(serie histórica de 2018 a 2022)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tasa de mortalidad materna, según dominio de estudio </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(serie histórica de 2018 a 2022)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Defunciones por sexo y Pueblo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, según 10 principales causas de muerte </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(comparar 2018 y 2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tasa de alfabetismo en la población de 15 años o más por sexo, según dominio de estudio </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(comparar 2018 y 2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nivel educativo de la población de 15 años o más por sexo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tasa neta </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>de escolaridad en el nivel primario por sexo (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>serie histórica de 2018 a 2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tasa neta de escolaridad en el nivel primario por sexo, según departamento</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tasa neta de escolaridad en el ciclo básico por sexo (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>serie histórica de 2018 a 2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tasa neta de escolaridad en el ciclo básico por sexo, según departamento </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tasa neta de escolaridad en el ciclo diversificado por sexo (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>serie histórica de 2018 a 2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tasa neta de escolaridad en el ciclo diversificado por sexo, según departamento</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tasa de deserción en el nivel primario por sexo (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>serie histórica de 2018 a 2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tasa de deserción en el nivel primario por sexo, según departamento</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tasa de deserción en el nivel básico por sexo (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>serie histórica de 2018 a 2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tasa de deserción en el nivel básico por sexo, según departamento</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tasa de deserción en el ciclo diversificado por sexo (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>serie histórica de 2018 a 2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tasa de deserción en el nivel diversificado por sexo, según departamento</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Proporción de la población matriculada en la universidad por sexo, según tipo de universidad (pública o privada)</t>
+  </si>
+  <si>
+    <t>Proporción de la población matriculada en la universidad pública por sexo, según campo de estudio</t>
+  </si>
+  <si>
+    <t>Proporción de la población matriculada en universidades privadas por sexo, según campo de estudio</t>
+  </si>
+  <si>
+    <t>Proporción de la población graduada de la universidad por sexo, según tipo de universidad (pública o privada)</t>
+  </si>
+  <si>
+    <t>Proporción de la población graduada de la universidad pública por sexo, según campo de estudio</t>
+  </si>
+  <si>
+    <r>
+      <t>Proporción de la población graduada de universidades privadas por sexo, según campo de estudio</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Acceso a la tecnología por sexo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ODS)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Carga global de trabajo entre las personas ocupadas de 15 años y más por sexo </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(comparar 2018 y 2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Carga global de trabajo de la población de 7 años o más, por sexo, según Pueblos, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(comparar 2018 y 2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tasa de participación económica por dominio de estudio, según sexo y estado conyugal </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(serie histórica de 2018 a 2022)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Población económicamente activa por sexo, según dominio de estudio</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(comparar 2018 y 2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Población económicamente activa por sexo, según Pueblos y grupos de edad </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(comparar 2018 y 2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Población económicamente activa por sexo, según dominio de estudio y sector económico</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Población ocupada por sexo, según rango de edad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Población ocupada por sexo, según dominio de estudio y categoría ocupacional</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Porcentaje de trabajadoras(es) afiliadas(os) al seguro social, según rama de actividad </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(comparar 2018 y 2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Créditos otorgados a la pequeña y mediana empresa por sexo </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(comparar 2018 y 2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Créditos otorgados a la pequeña y mediana empresa por sexo, según rama de actividad económica </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(comparar 2018 y 2022)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Salario o ingresos promedio por sexo, según dominio de estudio y rama de actividad económica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Salarios o ingresos promedio, desagregado por sexo, según pueblo</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tasa de desempleo en la población de 15 años o más por sexo, según dominio de estudio </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(comparar 2018 y 2022)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tasa desempleo en la población de 15 años o más por sexo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, según Pueblos </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(comparar 2018 y 2022)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mujeres jefas de hogar por número de hijas/hijos en la PO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Promedio de horas dedicadas a tareas domésticas no remuneradas por sexo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (ODS)</t>
+    </r>
+  </si>
+  <si>
+    <t>Distribución de tareas no remuneradas en el hogar por sexo</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tasa de matrimonios infantiles por sexo </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(serie histórica de 2018 a 2022)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Denuncias de violencia intrafamiliar por sexo, según tipo de agresión sufrida</t>
+  </si>
+  <si>
+    <t>Denuncias de violencia intrafamiliar por sexo, según grupos de edad</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Víctimas de violencia intrafamiliar por sexo </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(serie histórica de 2018 a 2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Víctimas de violencia intrafamiliar por sexo, según Pueblos </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(serie histórica de 2018 a 2022)</t>
+    </r>
+  </si>
+  <si>
+    <t>Víctimas de violencia intrafamiliar por sexo, según tipo de agresión sufrida (serie histórica de 2018 a 2022)</t>
+  </si>
+  <si>
+    <t>Instituciones que prestan atención a víctimas de violencia intrafamiliar, según tipo de servicio brindado (período 2018 - 2022)</t>
+  </si>
+  <si>
+    <t>Tasa promedio de denuncia por los delitos contemplado en la Ley Contra el Femicidio y Otras Formas de Violencia Contra a la Mujer, por departamento de registro (periodo 2020, 2021, 2022)</t>
+  </si>
+  <si>
+    <t>Muertes violentas por sexo, según causa de muerte y grupos de edad (comparar 2018 y 2022)</t>
+  </si>
+  <si>
+    <t>Número de muertes violentas de mujeres relacionadas con hechos delictivos (período 2018 - 2022)</t>
+  </si>
+  <si>
+    <r>
+      <t>Índice de mortalidad femenina (período 2018 - 2022)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mujeres privadas de libertad por tipo de delito (período 2018 - 2022)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Participación porcentual en los Consejos de Desarrollo por sexo, según cargo (compara 2018 y 2022)</t>
+  </si>
+  <si>
+    <t>Participación porcentual en los Consejos de Desarrollo por sexo, según cargo (comparar 2020 y 2021)</t>
+  </si>
+  <si>
+    <t>Porcentaje de Personas electas para el Organismo Legislativo por sexo (últimos tres años electorales)</t>
+  </si>
+  <si>
+    <t>Cantidad y porcentaje de mujeres en el gabinete ministerial (serie histórica 2018-2022)</t>
+  </si>
+  <si>
+    <t>Cantidad y porcentaje de mujeres en el Secretarías de la Presidencia de la República (serie histórica 2018-2022)</t>
+  </si>
+  <si>
+    <t>Cantidad y porcentaje de participación de mujeres en las alcaldías (serie histórica 2018-2022)</t>
+  </si>
+  <si>
+    <t>Porcentaje mujeres empadronadas (últimos tres años electorales)</t>
+  </si>
+  <si>
+    <t>Índice de feminidad en el padrón electoral (serie histórica 2018-2022)</t>
+  </si>
+  <si>
+    <t>Porcentaje de la población que votó con relación al total de empadronados (últimos tres años electorales)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -529,14 +2022,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -559,8 +2044,74 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF2F5496"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF2F5496"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FF2F5496"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -588,6 +2139,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8FE2FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -627,10 +2184,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -645,7 +2203,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -653,11 +2210,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -667,12 +2220,60 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF8FE2FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -982,10 +2583,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1F1446-4590-4473-8B94-EB49B6294D9F}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,14 +2618,14 @@
         <v>102</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>59</v>
       </c>
       <c r="D2" t="s">
@@ -1034,14 +2635,14 @@
         <v>90</v>
       </c>
       <c r="G2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="13"/>
       <c r="D3" t="s">
         <v>64</v>
       </c>
@@ -1049,14 +2650,14 @@
         <v>90</v>
       </c>
       <c r="G3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="13"/>
       <c r="D4" t="s">
         <v>64</v>
       </c>
@@ -1064,14 +2665,14 @@
         <v>90</v>
       </c>
       <c r="G4" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="13"/>
       <c r="D5" t="s">
         <v>64</v>
       </c>
@@ -1079,14 +2680,14 @@
         <v>90</v>
       </c>
       <c r="G5" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="13"/>
       <c r="D6" t="s">
         <v>64</v>
       </c>
@@ -1097,7 +2698,7 @@
         <v>115</v>
       </c>
       <c r="G6" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1114,7 +2715,7 @@
         <v>114</v>
       </c>
       <c r="G7" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1131,7 +2732,7 @@
         <v>116</v>
       </c>
       <c r="G8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1145,7 +2746,7 @@
         <v>90</v>
       </c>
       <c r="G9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1159,7 +2760,7 @@
         <v>90</v>
       </c>
       <c r="G10" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1173,7 +2774,7 @@
         <v>90</v>
       </c>
       <c r="G11" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1190,11 +2791,11 @@
         <v>91</v>
       </c>
       <c r="G12" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B13" t="s">
@@ -1210,7 +2811,7 @@
         <v>103</v>
       </c>
       <c r="G13" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1227,10 +2828,10 @@
         <v>67</v>
       </c>
       <c r="F14" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G14" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1247,10 +2848,10 @@
         <v>67</v>
       </c>
       <c r="F15" t="s">
-        <v>130</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>127</v>
+        <v>122</v>
+      </c>
+      <c r="G15" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1267,10 +2868,10 @@
         <v>67</v>
       </c>
       <c r="F16" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="G16" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1287,7 +2888,7 @@
         <v>67</v>
       </c>
       <c r="G17" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1304,7 +2905,7 @@
         <v>67</v>
       </c>
       <c r="G18" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1321,7 +2922,7 @@
         <v>67</v>
       </c>
       <c r="G19" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1338,7 +2939,7 @@
         <v>67</v>
       </c>
       <c r="G20" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1355,7 +2956,7 @@
         <v>67</v>
       </c>
       <c r="G21" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1372,7 +2973,7 @@
         <v>67</v>
       </c>
       <c r="G22" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1389,10 +2990,10 @@
         <v>67</v>
       </c>
       <c r="F23" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="G23" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1409,7 +3010,7 @@
         <v>67</v>
       </c>
       <c r="G24" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1426,7 +3027,7 @@
         <v>67</v>
       </c>
       <c r="G25" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1443,7 +3044,7 @@
         <v>67</v>
       </c>
       <c r="G26" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1460,7 +3061,7 @@
         <v>67</v>
       </c>
       <c r="G27" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1477,10 +3078,10 @@
         <v>67</v>
       </c>
       <c r="F28" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="G28" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1497,10 +3098,10 @@
         <v>67</v>
       </c>
       <c r="F29" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G29" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1517,7 +3118,7 @@
         <v>68</v>
       </c>
       <c r="G30" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1534,7 +3135,7 @@
         <v>68</v>
       </c>
       <c r="G31" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1551,7 +3152,7 @@
         <v>68</v>
       </c>
       <c r="G32" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1576,7 +3177,7 @@
         <v>68</v>
       </c>
       <c r="G34" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1593,7 +3194,7 @@
         <v>90</v>
       </c>
       <c r="G35" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1609,8 +3210,11 @@
       <c r="E36" t="s">
         <v>68</v>
       </c>
+      <c r="F36" t="s">
+        <v>153</v>
+      </c>
       <c r="G36" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1627,7 +3231,7 @@
         <v>68</v>
       </c>
       <c r="G37" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1644,7 +3248,7 @@
         <v>91</v>
       </c>
       <c r="G38" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -1661,11 +3265,11 @@
         <v>91</v>
       </c>
       <c r="G39" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B40" t="s">
@@ -1678,10 +3282,10 @@
         <v>91</v>
       </c>
       <c r="F40" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G40" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1698,7 +3302,7 @@
         <v>91</v>
       </c>
       <c r="G41" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -1715,11 +3319,11 @@
         <v>91</v>
       </c>
       <c r="G42" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B43" t="s">
@@ -1732,14 +3336,14 @@
         <v>91</v>
       </c>
       <c r="F43" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G43" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="10" t="s">
         <v>74</v>
       </c>
       <c r="B44" t="s">
@@ -1756,7 +3360,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B45" t="s">
@@ -1769,14 +3373,14 @@
         <v>91</v>
       </c>
       <c r="F45" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G45" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="7" t="s">
         <v>75</v>
       </c>
       <c r="B46" t="s">
@@ -1789,10 +3393,10 @@
         <v>91</v>
       </c>
       <c r="F46" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="G46" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1809,10 +3413,10 @@
         <v>91</v>
       </c>
       <c r="F47" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="G47" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1829,11 +3433,11 @@
         <v>91</v>
       </c>
       <c r="G48" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B49" t="s">
@@ -1846,10 +3450,10 @@
         <v>91</v>
       </c>
       <c r="F49" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="G49" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1866,11 +3470,11 @@
         <v>91</v>
       </c>
       <c r="G50" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="8" t="s">
         <v>76</v>
       </c>
       <c r="B51" t="s">
@@ -1883,14 +3487,14 @@
         <v>91</v>
       </c>
       <c r="F51" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="G51" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B52" t="s">
@@ -1903,13 +3507,13 @@
         <v>91</v>
       </c>
       <c r="F52" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="G52" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>41</v>
       </c>
@@ -1923,11 +3527,11 @@
         <v>91</v>
       </c>
       <c r="G53" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B54" t="s">
@@ -1940,10 +3544,10 @@
         <v>91</v>
       </c>
       <c r="F54" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G54" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1960,11 +3564,11 @@
         <v>91</v>
       </c>
       <c r="G55" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B56" t="s">
@@ -1977,14 +3581,14 @@
         <v>91</v>
       </c>
       <c r="F56" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="G56" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B57" t="s">
@@ -2003,12 +3607,12 @@
         <v>103</v>
       </c>
       <c r="G57" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B58" t="s">
         <v>84</v>
@@ -2020,12 +3624,12 @@
         <v>95</v>
       </c>
       <c r="G58" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B59" t="s">
         <v>84</v>
@@ -2037,7 +3641,7 @@
         <v>95</v>
       </c>
       <c r="G59" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -2054,11 +3658,11 @@
         <v>95</v>
       </c>
       <c r="G60" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="8" t="s">
+      <c r="A61" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B61" t="s">
@@ -2071,10 +3675,10 @@
         <v>95</v>
       </c>
       <c r="F61" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="G61" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -2091,7 +3695,7 @@
         <v>95</v>
       </c>
       <c r="G62" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -2108,11 +3712,11 @@
         <v>95</v>
       </c>
       <c r="G63" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="8" t="s">
+      <c r="A64" s="7" t="s">
         <v>98</v>
       </c>
       <c r="B64" t="s">
@@ -2125,10 +3729,10 @@
         <v>95</v>
       </c>
       <c r="F64" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="G64" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -2145,15 +3749,15 @@
         <v>95</v>
       </c>
       <c r="F65" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="G65" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B66" t="s">
         <v>84</v>
@@ -2165,7 +3769,7 @@
         <v>95</v>
       </c>
       <c r="G66" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -2182,12 +3786,12 @@
         <v>95</v>
       </c>
       <c r="G67" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B68" t="s">
         <v>78</v>
@@ -2199,7 +3803,7 @@
         <v>92</v>
       </c>
       <c r="G68" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2216,7 +3820,7 @@
         <v>92</v>
       </c>
       <c r="G69" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2233,7 +3837,7 @@
         <v>92</v>
       </c>
       <c r="G70" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2250,7 +3854,7 @@
         <v>92</v>
       </c>
       <c r="G71" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2267,7 +3871,7 @@
         <v>92</v>
       </c>
       <c r="G72" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2277,14 +3881,14 @@
       <c r="B73" t="s">
         <v>78</v>
       </c>
-      <c r="D73" s="6" t="s">
+      <c r="D73" s="28" t="s">
         <v>79</v>
       </c>
       <c r="E73" t="s">
         <v>92</v>
       </c>
       <c r="G73" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2301,7 +3905,7 @@
         <v>92</v>
       </c>
       <c r="G74" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2318,7 +3922,7 @@
         <v>92</v>
       </c>
       <c r="G75" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -2338,11 +3942,11 @@
         <v>67</v>
       </c>
       <c r="G76" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D77" t="s">
@@ -2352,14 +3956,14 @@
         <v>91</v>
       </c>
       <c r="F77" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="G77" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="6" t="s">
         <v>94</v>
       </c>
       <c r="D78" t="s">
@@ -2369,12 +3973,15 @@
         <v>95</v>
       </c>
       <c r="G78" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="7" t="s">
+      <c r="A79" s="6" t="s">
         <v>100</v>
+      </c>
+      <c r="B79" t="s">
+        <v>68</v>
       </c>
       <c r="D79" t="s">
         <v>68</v>
@@ -2383,14 +3990,14 @@
         <v>68</v>
       </c>
       <c r="F79" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="G79" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="7" t="s">
+      <c r="A80" s="6" t="s">
         <v>101</v>
       </c>
       <c r="D80" t="s">
@@ -2400,14 +4007,14 @@
         <v>95</v>
       </c>
       <c r="F80" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="G80" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="6" t="s">
         <v>105</v>
       </c>
       <c r="D81" t="s">
@@ -2416,12 +4023,15 @@
       <c r="E81" t="s">
         <v>90</v>
       </c>
+      <c r="F81" t="s">
+        <v>151</v>
+      </c>
       <c r="G81" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="7" t="s">
+      <c r="A82" s="6" t="s">
         <v>106</v>
       </c>
       <c r="D82" t="s">
@@ -2430,12 +4040,15 @@
       <c r="E82" t="s">
         <v>90</v>
       </c>
+      <c r="F82" t="s">
+        <v>151</v>
+      </c>
       <c r="G82" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="7" t="s">
+      <c r="A83" s="6" t="s">
         <v>108</v>
       </c>
       <c r="D83" t="s">
@@ -2445,13 +4058,14 @@
         <v>91</v>
       </c>
       <c r="G83" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
-        <v>110</v>
-      </c>
+      <c r="A84" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C84" s="9"/>
       <c r="D84" t="s">
         <v>65</v>
       </c>
@@ -2459,68 +4073,138 @@
         <v>91</v>
       </c>
       <c r="G84" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="7" t="s">
-        <v>110</v>
+      <c r="A85" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="D85" t="s">
         <v>65</v>
       </c>
       <c r="E85" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="G85" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C86" s="10"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="12" t="s">
+        <v>141</v>
+      </c>
       <c r="D86" t="s">
+        <v>85</v>
+      </c>
+      <c r="E86" t="s">
+        <v>95</v>
+      </c>
+      <c r="G86" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B87" t="s">
+        <v>68</v>
+      </c>
+      <c r="D87" t="s">
+        <v>147</v>
+      </c>
+      <c r="E87" t="s">
+        <v>68</v>
+      </c>
+      <c r="F87" t="s">
+        <v>148</v>
+      </c>
+      <c r="G87" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D88" t="s">
         <v>65</v>
       </c>
-      <c r="E86" t="s">
-        <v>91</v>
-      </c>
-      <c r="G86" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="E88" t="s">
+        <v>90</v>
+      </c>
+      <c r="F88" t="s">
+        <v>150</v>
+      </c>
+      <c r="G88" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E89" t="s">
+        <v>68</v>
+      </c>
+      <c r="F89" t="s">
+        <v>148</v>
+      </c>
+      <c r="G89" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D90" t="s">
+        <v>68</v>
+      </c>
+      <c r="E90" t="s">
+        <v>68</v>
+      </c>
+      <c r="F90" t="s">
+        <v>155</v>
+      </c>
+      <c r="G90" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D91" t="s">
+        <v>157</v>
+      </c>
+      <c r="E91" t="s">
+        <v>68</v>
+      </c>
+      <c r="F91" t="s">
+        <v>158</v>
+      </c>
+      <c r="G91" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D92" t="s">
         <v>65</v>
       </c>
-      <c r="E87" t="s">
-        <v>95</v>
-      </c>
-      <c r="G87" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="D88" t="s">
-        <v>85</v>
-      </c>
-      <c r="E88" t="s">
-        <v>95</v>
-      </c>
-      <c r="G88" t="s">
-        <v>127</v>
+      <c r="E92" t="s">
+        <v>90</v>
+      </c>
+      <c r="G92" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G88" xr:uid="{0A1F1446-4590-4473-8B94-EB49B6294D9F}">
+  <autoFilter ref="A1:G92" xr:uid="{0A1F1446-4590-4473-8B94-EB49B6294D9F}">
     <filterColumn colId="4">
       <filters>
         <filter val="Participación Política"/>
@@ -2536,80 +4220,1038 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1B3959-296E-464C-92E4-F60B9525B2A5}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65DEFAE6-4843-4FD7-A153-29A19AA5AB96}">
+  <dimension ref="A1:C146"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="95.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="184.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>102</v>
+    <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2">
-        <v>2007</v>
+      <c r="A2" s="27"/>
+      <c r="B2" s="25">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3">
-        <v>2008</v>
+      <c r="A3" s="27"/>
+      <c r="B3" s="25">
+        <v>1.2</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4">
-        <v>2008</v>
+      <c r="A4" s="27"/>
+      <c r="B4" s="25">
+        <v>1.3</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B5">
-        <v>2008</v>
+      <c r="A5" s="27"/>
+      <c r="B5" s="25">
+        <v>1.4</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B6">
-        <v>2013</v>
+      <c r="A6" s="27"/>
+      <c r="B6" s="25">
+        <v>1.5</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B7">
-        <v>2013</v>
+      <c r="A7" s="27"/>
+      <c r="B7" s="25">
+        <v>1.6</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="25">
+        <v>1.7</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="25">
+        <v>1.8</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1.9</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="20">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1.17</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>2.1</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>2.4</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>2.5</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>2.6</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>2.7</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>2.8</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>2.9</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="20">
+        <v>2.1</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>2.11</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>2.12</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="23" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>3.1</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <f>B33+0.1</f>
+        <v>3.2</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <f t="shared" ref="B35:B41" si="0">B34+0.1</f>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>3.5000000000000004</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>3.6000000000000005</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>3.7000000000000006</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>3.8000000000000007</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>3.9000000000000008</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="20">
+        <v>3.1</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="20">
+        <f>B42+0.01</f>
+        <v>3.11</v>
+      </c>
+      <c r="C43" s="22" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="20">
+        <f t="shared" ref="B44:B53" si="1">B43+0.01</f>
+        <v>3.1199999999999997</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="20">
+        <f t="shared" si="1"/>
+        <v>3.1299999999999994</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="20">
+        <f t="shared" si="1"/>
+        <v>3.1399999999999992</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="20">
+        <f t="shared" si="1"/>
+        <v>3.149999999999999</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B48" s="20">
+        <f t="shared" si="1"/>
+        <v>3.1599999999999988</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="20">
+        <f t="shared" si="1"/>
+        <v>3.1699999999999986</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="20">
+        <f t="shared" si="1"/>
+        <v>3.1799999999999984</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B51" s="20">
+        <f t="shared" si="1"/>
+        <v>3.1899999999999982</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B52" s="20">
+        <f t="shared" si="1"/>
+        <v>3.199999999999998</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B53" s="20">
+        <f t="shared" si="1"/>
+        <v>3.2099999999999977</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A54" s="23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <f>B55+0.1</f>
+        <v>4.1999999999999993</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <f t="shared" ref="B57:B63" si="2">B56+0.1</f>
+        <v>4.2999999999999989</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <f t="shared" si="2"/>
+        <v>4.3999999999999986</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <f t="shared" si="2"/>
+        <v>4.4999999999999982</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <f t="shared" si="2"/>
+        <v>4.5999999999999979</v>
+      </c>
+      <c r="C60" s="22" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <f t="shared" si="2"/>
+        <v>4.6999999999999975</v>
+      </c>
+      <c r="C61" s="22" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <f t="shared" si="2"/>
+        <v>4.7999999999999972</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <f t="shared" si="2"/>
+        <v>4.8999999999999968</v>
+      </c>
+      <c r="C63" s="22" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B64" s="20">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <f t="shared" ref="B65:B73" si="3">B64+0.01</f>
+        <v>4.1099999999999994</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <f t="shared" si="3"/>
+        <v>4.1199999999999992</v>
+      </c>
+      <c r="C66" s="22" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <f t="shared" si="3"/>
+        <v>4.129999999999999</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <f t="shared" si="3"/>
+        <v>4.1399999999999988</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <f t="shared" si="3"/>
+        <v>4.1499999999999986</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <f t="shared" si="3"/>
+        <v>4.1599999999999984</v>
+      </c>
+      <c r="C70" s="22" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <f t="shared" si="3"/>
+        <v>4.1699999999999982</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <f t="shared" si="3"/>
+        <v>4.1799999999999979</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <f t="shared" si="3"/>
+        <v>4.1899999999999977</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C74" s="16"/>
+    </row>
+    <row r="75" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A75" s="23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C76" s="22" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <f>B76+0.1</f>
+        <v>5.1999999999999993</v>
+      </c>
+      <c r="C77" s="22" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <f t="shared" ref="B78:B84" si="4">B77+0.1</f>
+        <v>5.2999999999999989</v>
+      </c>
+      <c r="C78" s="22" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <f t="shared" si="4"/>
+        <v>5.3999999999999986</v>
+      </c>
+      <c r="C79" s="22" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <f t="shared" si="4"/>
+        <v>5.4999999999999982</v>
+      </c>
+      <c r="C80" s="22" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <f t="shared" si="4"/>
+        <v>5.5999999999999979</v>
+      </c>
+      <c r="C81" s="22" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <f t="shared" si="4"/>
+        <v>5.6999999999999975</v>
+      </c>
+      <c r="C82" s="22" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <f t="shared" si="4"/>
+        <v>5.7999999999999972</v>
+      </c>
+      <c r="C83" s="22" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <f t="shared" si="4"/>
+        <v>5.8999999999999968</v>
+      </c>
+      <c r="C84" s="22" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B85" s="20">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C85" s="22" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <f t="shared" ref="B86:B87" si="5">B85+0.01</f>
+        <v>5.1099999999999994</v>
+      </c>
+      <c r="C86" s="22" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <f t="shared" si="5"/>
+        <v>5.1199999999999992</v>
+      </c>
+      <c r="C87" s="22" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A88" s="23" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>6.1</v>
+      </c>
+      <c r="C89" s="22" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <f>B89+0.1</f>
+        <v>6.1999999999999993</v>
+      </c>
+      <c r="C90" s="22" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <f t="shared" ref="B91:B97" si="6">B90+0.1</f>
+        <v>6.2999999999999989</v>
+      </c>
+      <c r="C91" s="22" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <f t="shared" si="6"/>
+        <v>6.3999999999999986</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <f t="shared" si="6"/>
+        <v>6.4999999999999982</v>
+      </c>
+      <c r="C93" s="22" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <f t="shared" si="6"/>
+        <v>6.5999999999999979</v>
+      </c>
+      <c r="C94" s="22" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <f t="shared" si="6"/>
+        <v>6.6999999999999975</v>
+      </c>
+      <c r="C95" s="22" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <f t="shared" si="6"/>
+        <v>6.7999999999999972</v>
+      </c>
+      <c r="C96" s="22" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <f t="shared" si="6"/>
+        <v>6.8999999999999968</v>
+      </c>
+      <c r="C97" s="22" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B98" s="20"/>
+      <c r="C98" s="15"/>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C99" s="17"/>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="17"/>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C101" s="17"/>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C102" s="17"/>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C103" s="17"/>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C104" s="17"/>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C105" s="18"/>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C106" s="17"/>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C107" s="17"/>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C108" s="18"/>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C109" s="17"/>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C110" s="18"/>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C111" s="17"/>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C112" s="17"/>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C113" s="17"/>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C114" s="17"/>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C115" s="18"/>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C116" s="17"/>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C117" s="17"/>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C118" s="18"/>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C120" s="17"/>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C121" s="17" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C122" s="17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C123" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C124" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C125" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C126" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C127" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C128" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C129" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C130" s="17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C131" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C132" s="19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C133" s="17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C134" s="17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C135" s="17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C136" s="17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C137" s="17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C138" s="17" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C139" s="17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C140" s="17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C141" s="17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C142" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C143" s="17" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C144" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C145" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C146" s="17" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A9"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C132" r:id="rId1" display="http://pnd.gt/Home/goals?code=ODS5" xr:uid="{9753D7AD-147F-4A0C-BDC8-F0D45EB9757D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambio listado fuentes Excel
</commit_message>
<xml_diff>
--- a/Listado Indicadores/Listado de indicadores a trabajar.xlsx
+++ b/Listado Indicadores/Listado de indicadores a trabajar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inegobgt-my.sharepoint.com/personal/pgalvez_ine_gob_gt/Documents/Documentos/GitHub/CompendioGenero2023/Listado Indicadores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="421" documentId="8_{33C4EBF3-B6E3-430A-80A9-911051E32003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D225325-2E87-49B9-A059-D9A04F5B6D22}"/>
+  <xr:revisionPtr revIDLastSave="424" documentId="8_{33C4EBF3-B6E3-430A-80A9-911051E32003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA4D750C-3658-4905-811A-8BBFC451E755}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3D4A4D73-1AC6-4F09-9897-696579B6A714}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="261">
   <si>
     <t>Distribución de la población total por sexo según grupo de edad</t>
   </si>
@@ -259,9 +259,6 @@
   </si>
   <si>
     <t>MINECO programa MIPYME</t>
-  </si>
-  <si>
-    <t>INE</t>
   </si>
   <si>
     <t>Distribución porcentual de la población ocupada, por  area geografica según categoria ocupacional y por sexo</t>
@@ -2188,7 +2185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2219,9 +2216,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -2258,10 +2252,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2582,11 +2578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1F1446-4590-4473-8B94-EB49B6294D9F}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2600,7 +2595,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>56</v>
@@ -2612,96 +2607,96 @@
         <v>58</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="26" t="s">
         <v>59</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="26"/>
       <c r="D3" t="s">
         <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="13"/>
+      <c r="B4" s="26"/>
       <c r="D4" t="s">
         <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="13"/>
+      <c r="B5" s="26"/>
       <c r="D5" t="s">
         <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="13"/>
+      <c r="B6" s="26"/>
       <c r="D6" t="s">
         <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -2709,16 +2704,16 @@
         <v>65</v>
       </c>
       <c r="E7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
@@ -2726,16 +2721,16 @@
         <v>65</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -2743,13 +2738,13 @@
         <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -2757,27 +2752,27 @@
         <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11" t="s">
         <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -2788,13 +2783,13 @@
         <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>6</v>
       </c>
@@ -2805,16 +2800,16 @@
         <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -2828,13 +2823,13 @@
         <v>67</v>
       </c>
       <c r="F14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -2848,13 +2843,13 @@
         <v>67</v>
       </c>
       <c r="F15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G15" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -2868,13 +2863,13 @@
         <v>67</v>
       </c>
       <c r="F16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G16" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -2888,10 +2883,10 @@
         <v>67</v>
       </c>
       <c r="G17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
@@ -2905,10 +2900,10 @@
         <v>67</v>
       </c>
       <c r="G18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -2922,10 +2917,10 @@
         <v>67</v>
       </c>
       <c r="G19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -2939,10 +2934,10 @@
         <v>67</v>
       </c>
       <c r="G20" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -2956,10 +2951,10 @@
         <v>67</v>
       </c>
       <c r="G21" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
@@ -2973,10 +2968,10 @@
         <v>67</v>
       </c>
       <c r="G22" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
@@ -2990,13 +2985,13 @@
         <v>67</v>
       </c>
       <c r="F23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G23" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
@@ -3010,10 +3005,10 @@
         <v>67</v>
       </c>
       <c r="G24" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
@@ -3027,10 +3022,10 @@
         <v>67</v>
       </c>
       <c r="G25" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
@@ -3044,10 +3039,10 @@
         <v>67</v>
       </c>
       <c r="G26" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>20</v>
       </c>
@@ -3061,10 +3056,10 @@
         <v>67</v>
       </c>
       <c r="G27" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -3078,13 +3073,13 @@
         <v>67</v>
       </c>
       <c r="F28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G28" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
@@ -3098,13 +3093,13 @@
         <v>67</v>
       </c>
       <c r="F29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G29" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -3118,10 +3113,10 @@
         <v>68</v>
       </c>
       <c r="G30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
@@ -3135,10 +3130,10 @@
         <v>68</v>
       </c>
       <c r="G31" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -3152,10 +3147,10 @@
         <v>68</v>
       </c>
       <c r="G32" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -3166,7 +3161,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>27</v>
       </c>
@@ -3177,10 +3172,10 @@
         <v>68</v>
       </c>
       <c r="G34" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>28</v>
       </c>
@@ -3191,13 +3186,13 @@
         <v>64</v>
       </c>
       <c r="E35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G35" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>29</v>
       </c>
@@ -3211,13 +3206,13 @@
         <v>68</v>
       </c>
       <c r="F36" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G36" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>30</v>
       </c>
@@ -3231,579 +3226,579 @@
         <v>68</v>
       </c>
       <c r="G37" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D38" t="s">
         <v>65</v>
       </c>
       <c r="E38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G38" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D39" t="s">
         <v>65</v>
       </c>
       <c r="E39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G39" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G40" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D41" t="s">
         <v>72</v>
       </c>
       <c r="E41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G41" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D42" t="s">
         <v>72</v>
       </c>
       <c r="E42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G42" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D43" t="s">
         <v>65</v>
       </c>
       <c r="E43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G43" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D44" t="s">
         <v>65</v>
       </c>
       <c r="E44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F44" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D45" t="s">
         <v>65</v>
       </c>
       <c r="E45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G45" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D46" t="s">
         <v>65</v>
       </c>
       <c r="E46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G46" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B47" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" t="s">
         <v>86</v>
       </c>
-      <c r="D47" t="s">
-        <v>87</v>
-      </c>
       <c r="E47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G47" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D48" t="s">
         <v>65</v>
       </c>
       <c r="E48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G48" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D49" t="s">
         <v>65</v>
       </c>
       <c r="E49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G49" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B50" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D50" t="s">
         <v>65</v>
       </c>
       <c r="E50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G50" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B51" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D51" t="s">
         <v>65</v>
       </c>
       <c r="E51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F51" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G51" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D52" t="s">
         <v>65</v>
       </c>
       <c r="E52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G52" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B53" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D53" t="s">
         <v>65</v>
       </c>
       <c r="E53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G53" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D54" t="s">
         <v>65</v>
       </c>
       <c r="E54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F54" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G54" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D55" t="s">
         <v>65</v>
       </c>
       <c r="E55" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G55" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D56" t="s">
         <v>65</v>
       </c>
       <c r="E56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G56" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C57">
         <v>5.4</v>
       </c>
       <c r="D57" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E57" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G57" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B58" t="s">
+        <v>83</v>
+      </c>
+      <c r="D58" t="s">
+        <v>84</v>
+      </c>
+      <c r="E58" t="s">
+        <v>94</v>
+      </c>
+      <c r="G58" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
+        <v>83</v>
+      </c>
+      <c r="D59" t="s">
         <v>84</v>
       </c>
-      <c r="D58" t="s">
-        <v>85</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="E59" t="s">
+        <v>94</v>
+      </c>
+      <c r="G59" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G58" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
+        <v>83</v>
+      </c>
+      <c r="D60" t="s">
         <v>84</v>
       </c>
-      <c r="D59" t="s">
-        <v>85</v>
-      </c>
-      <c r="E59" t="s">
-        <v>95</v>
-      </c>
-      <c r="G59" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B60" t="s">
-        <v>84</v>
-      </c>
-      <c r="D60" t="s">
-        <v>85</v>
-      </c>
       <c r="E60" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G60" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B61" t="s">
+        <v>83</v>
+      </c>
+      <c r="D61" t="s">
         <v>84</v>
       </c>
-      <c r="D61" t="s">
-        <v>85</v>
-      </c>
       <c r="E61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F61" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G61" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B62" t="s">
+        <v>83</v>
+      </c>
+      <c r="D62" t="s">
         <v>84</v>
       </c>
-      <c r="D62" t="s">
-        <v>85</v>
-      </c>
       <c r="E62" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G62" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B63" t="s">
+        <v>83</v>
+      </c>
+      <c r="D63" t="s">
+        <v>84</v>
+      </c>
+      <c r="E63" t="s">
+        <v>94</v>
+      </c>
+      <c r="G63" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
+        <v>83</v>
+      </c>
+      <c r="D64" t="s">
         <v>84</v>
       </c>
-      <c r="D63" t="s">
-        <v>85</v>
-      </c>
-      <c r="E63" t="s">
-        <v>95</v>
-      </c>
-      <c r="G63" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
+      <c r="E64" t="s">
+        <v>94</v>
+      </c>
+      <c r="F64" t="s">
+        <v>138</v>
+      </c>
+      <c r="G64" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B64" t="s">
-        <v>84</v>
-      </c>
-      <c r="D64" t="s">
-        <v>85</v>
-      </c>
-      <c r="E64" t="s">
-        <v>95</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="B65" t="s">
+        <v>83</v>
+      </c>
+      <c r="D65" t="s">
+        <v>82</v>
+      </c>
+      <c r="E65" t="s">
+        <v>94</v>
+      </c>
+      <c r="F65" t="s">
         <v>139</v>
       </c>
-      <c r="G64" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B65" t="s">
-        <v>84</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="G65" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B66" t="s">
         <v>83</v>
       </c>
-      <c r="E65" t="s">
-        <v>95</v>
-      </c>
-      <c r="F65" t="s">
-        <v>140</v>
-      </c>
-      <c r="G65" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B66" t="s">
-        <v>84</v>
-      </c>
       <c r="D66" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E66" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G66" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B67" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D67" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G67" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B68" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E68" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G68" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3811,16 +3806,16 @@
         <v>49</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D69" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E69" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G69" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -3828,16 +3823,16 @@
         <v>50</v>
       </c>
       <c r="B70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D70" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G70" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3845,16 +3840,16 @@
         <v>51</v>
       </c>
       <c r="B71" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D71" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E71" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G71" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3862,16 +3857,16 @@
         <v>52</v>
       </c>
       <c r="B72" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D72" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E72" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G72" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3879,16 +3874,16 @@
         <v>53</v>
       </c>
       <c r="B73" t="s">
+        <v>77</v>
+      </c>
+      <c r="D73" t="s">
         <v>78</v>
       </c>
-      <c r="D73" s="28" t="s">
-        <v>79</v>
-      </c>
       <c r="E73" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G73" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3896,16 +3891,16 @@
         <v>54</v>
       </c>
       <c r="B74" t="s">
+        <v>77</v>
+      </c>
+      <c r="D74" t="s">
         <v>78</v>
       </c>
-      <c r="D74" t="s">
-        <v>79</v>
-      </c>
       <c r="E74" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G74" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3913,27 +3908,27 @@
         <v>55</v>
       </c>
       <c r="B75" t="s">
+        <v>77</v>
+      </c>
+      <c r="D75" t="s">
         <v>78</v>
       </c>
-      <c r="D75" t="s">
-        <v>79</v>
-      </c>
       <c r="E75" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G75" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B76" t="s">
         <v>67</v>
       </c>
       <c r="C76" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D76" t="s">
         <v>65</v>
@@ -3942,43 +3937,43 @@
         <v>67</v>
       </c>
       <c r="G76" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D77" t="s">
         <v>65</v>
       </c>
       <c r="E77" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F77" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G77" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D78" t="s">
+        <v>103</v>
+      </c>
+      <c r="E78" t="s">
         <v>94</v>
       </c>
-      <c r="D78" t="s">
-        <v>104</v>
-      </c>
-      <c r="E78" t="s">
-        <v>95</v>
-      </c>
       <c r="G78" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B79" t="s">
         <v>68</v>
@@ -3990,174 +3985,174 @@
         <v>68</v>
       </c>
       <c r="F79" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G79" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D80" t="s">
+        <v>103</v>
+      </c>
+      <c r="E80" t="s">
+        <v>94</v>
+      </c>
+      <c r="F80" t="s">
+        <v>142</v>
+      </c>
+      <c r="G80" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E80" t="s">
-        <v>95</v>
-      </c>
-      <c r="F80" t="s">
-        <v>143</v>
-      </c>
-      <c r="G80" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="s">
+      <c r="D81" t="s">
+        <v>108</v>
+      </c>
+      <c r="E81" t="s">
+        <v>89</v>
+      </c>
+      <c r="F81" t="s">
+        <v>150</v>
+      </c>
+      <c r="G81" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D81" t="s">
-        <v>109</v>
-      </c>
-      <c r="E81" t="s">
-        <v>90</v>
-      </c>
-      <c r="F81" t="s">
-        <v>151</v>
-      </c>
-      <c r="G81" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="6" t="s">
-        <v>106</v>
-      </c>
       <c r="D82" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E82" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F82" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G82" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D83" t="s">
         <v>65</v>
       </c>
       <c r="E83" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G83" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C84" s="9"/>
       <c r="D84" t="s">
         <v>65</v>
       </c>
       <c r="E84" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G84" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D85" t="s">
         <v>65</v>
       </c>
       <c r="E85" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G85" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D86" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E86" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G86" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B87" t="s">
         <v>68</v>
       </c>
       <c r="D87" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E87" t="s">
         <v>68</v>
       </c>
       <c r="F87" t="s">
+        <v>147</v>
+      </c>
+      <c r="G87" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="G87" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>149</v>
       </c>
       <c r="D88" t="s">
         <v>65</v>
       </c>
       <c r="E88" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F88" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G88" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E89" t="s">
         <v>68</v>
       </c>
       <c r="F89" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G89" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D90" t="s">
         <v>68</v>
@@ -4166,51 +4161,45 @@
         <v>68</v>
       </c>
       <c r="F90" t="s">
+        <v>154</v>
+      </c>
+      <c r="G90" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="G90" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
+      <c r="D91" t="s">
         <v>156</v>
-      </c>
-      <c r="D91" t="s">
-        <v>157</v>
       </c>
       <c r="E91" t="s">
         <v>68</v>
       </c>
       <c r="F91" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G91" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D92" t="s">
         <v>65</v>
       </c>
       <c r="E92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G92" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G92" xr:uid="{0A1F1446-4590-4473-8B94-EB49B6294D9F}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Participación Política"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G92" xr:uid="{0A1F1446-4590-4473-8B94-EB49B6294D9F}"/>
   <mergeCells count="1">
     <mergeCell ref="B2:B6"/>
   </mergeCells>
@@ -4234,111 +4223,111 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>159</v>
+      <c r="A1" s="13" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
-      <c r="B2" s="25">
+      <c r="B2" s="24">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>177</v>
+      <c r="C2" s="25" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
-      <c r="B3" s="25">
+      <c r="B3" s="24">
         <v>1.2</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>178</v>
+      <c r="C3" s="25" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
-      <c r="B4" s="25">
+      <c r="B4" s="24">
         <v>1.3</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>179</v>
+      <c r="C4" s="25" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="27"/>
-      <c r="B5" s="25">
+      <c r="B5" s="24">
         <v>1.4</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="25" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
-      <c r="B6" s="25">
+      <c r="B6" s="24">
         <v>1.5</v>
       </c>
-      <c r="C6" s="26" t="s">
-        <v>180</v>
+      <c r="C6" s="25" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="27"/>
-      <c r="B7" s="25">
+      <c r="B7" s="24">
         <v>1.6</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>181</v>
+      <c r="C7" s="25" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="27"/>
-      <c r="B8" s="25">
+      <c r="B8" s="24">
         <v>1.7</v>
       </c>
-      <c r="C8" s="26" t="s">
-        <v>182</v>
+      <c r="C8" s="25" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
-      <c r="B9" s="25">
+      <c r="B9" s="24">
         <v>1.8</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>183</v>
+      <c r="C9" s="25" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1.9</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="20" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C11" s="20" t="s">
         <v>184</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="20">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>1.1100000000000001</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>186</v>
+      <c r="C12" s="20" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4346,154 +4335,154 @@
       <c r="B14">
         <v>1.1299999999999999</v>
       </c>
-      <c r="C14" s="21" t="s">
-        <v>187</v>
+      <c r="C14" s="20" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>1.1399999999999999</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>188</v>
+      <c r="C15" s="20" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>1.1499999999999999</v>
       </c>
-      <c r="C16" s="21" t="s">
-        <v>189</v>
+      <c r="C16" s="20" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>1.1599999999999999</v>
       </c>
-      <c r="C17" s="21" t="s">
-        <v>190</v>
+      <c r="C17" s="20" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>1.17</v>
       </c>
-      <c r="C18" s="22" t="s">
-        <v>191</v>
+      <c r="C18" s="21" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>160</v>
+      <c r="A19" s="13" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>2.1</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>192</v>
+      <c r="C20" s="21" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C21" s="22" t="s">
-        <v>154</v>
+      <c r="C21" s="21" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C22" s="22" t="s">
-        <v>193</v>
+      <c r="C22" s="21" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>2.4</v>
       </c>
-      <c r="C23" s="22" t="s">
-        <v>194</v>
+      <c r="C23" s="21" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>2.5</v>
       </c>
-      <c r="C24" s="22" t="s">
-        <v>195</v>
+      <c r="C24" s="21" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>2.6</v>
       </c>
-      <c r="C25" s="22" t="s">
-        <v>196</v>
+      <c r="C25" s="21" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>2.7</v>
       </c>
-      <c r="C26" s="22" t="s">
-        <v>197</v>
+      <c r="C26" s="21" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>2.8</v>
       </c>
-      <c r="C27" s="22" t="s">
-        <v>198</v>
+      <c r="C27" s="21" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>2.9</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="19">
+        <v>2.1</v>
+      </c>
+      <c r="C29" s="21" t="s">
         <v>199</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="20">
-        <v>2.1</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>2.11</v>
       </c>
-      <c r="C30" s="22" t="s">
-        <v>156</v>
+      <c r="C30" s="21" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>2.12</v>
       </c>
-      <c r="C31" s="22" t="s">
-        <v>201</v>
+      <c r="C31" s="21" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
-        <v>161</v>
+      <c r="A32" s="22" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>3.1</v>
       </c>
-      <c r="C33" s="22" t="s">
-        <v>202</v>
+      <c r="C33" s="21" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4501,8 +4490,8 @@
         <f>B33+0.1</f>
         <v>3.2</v>
       </c>
-      <c r="C34" s="24" t="s">
-        <v>203</v>
+      <c r="C34" s="23" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4510,8 +4499,8 @@
         <f t="shared" ref="B35:B41" si="0">B34+0.1</f>
         <v>3.3000000000000003</v>
       </c>
-      <c r="C35" s="22" t="s">
-        <v>204</v>
+      <c r="C35" s="21" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4519,8 +4508,8 @@
         <f t="shared" si="0"/>
         <v>3.4000000000000004</v>
       </c>
-      <c r="C36" s="22" t="s">
-        <v>205</v>
+      <c r="C36" s="21" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4528,8 +4517,8 @@
         <f t="shared" si="0"/>
         <v>3.5000000000000004</v>
       </c>
-      <c r="C37" s="22" t="s">
-        <v>206</v>
+      <c r="C37" s="21" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4537,8 +4526,8 @@
         <f t="shared" si="0"/>
         <v>3.6000000000000005</v>
       </c>
-      <c r="C38" s="22" t="s">
-        <v>207</v>
+      <c r="C38" s="21" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4546,8 +4535,8 @@
         <f t="shared" si="0"/>
         <v>3.7000000000000006</v>
       </c>
-      <c r="C39" s="22" t="s">
-        <v>208</v>
+      <c r="C39" s="21" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="40" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4555,8 +4544,8 @@
         <f t="shared" si="0"/>
         <v>3.8000000000000007</v>
       </c>
-      <c r="C40" s="22" t="s">
-        <v>209</v>
+      <c r="C40" s="21" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4564,127 +4553,127 @@
         <f t="shared" si="0"/>
         <v>3.9000000000000008</v>
       </c>
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="19">
+        <v>3.1</v>
+      </c>
+      <c r="C42" s="21" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="42" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B42" s="20">
-        <v>3.1</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>211</v>
-      </c>
-    </row>
     <row r="43" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="20">
+      <c r="B43" s="19">
         <f>B42+0.01</f>
         <v>3.11</v>
       </c>
-      <c r="C43" s="22" t="s">
-        <v>212</v>
+      <c r="C43" s="21" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="20">
+      <c r="B44" s="19">
         <f t="shared" ref="B44:B53" si="1">B43+0.01</f>
         <v>3.1199999999999997</v>
       </c>
-      <c r="C44" s="22" t="s">
-        <v>213</v>
+      <c r="C44" s="21" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="45" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B45" s="20">
+      <c r="B45" s="19">
         <f t="shared" si="1"/>
         <v>3.1299999999999994</v>
       </c>
-      <c r="C45" s="22" t="s">
-        <v>214</v>
+      <c r="C45" s="21" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="46" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B46" s="20">
+      <c r="B46" s="19">
         <f t="shared" si="1"/>
         <v>3.1399999999999992</v>
       </c>
-      <c r="C46" s="22" t="s">
-        <v>215</v>
+      <c r="C46" s="21" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="20">
+      <c r="B47" s="19">
         <f t="shared" si="1"/>
         <v>3.149999999999999</v>
       </c>
-      <c r="C47" s="22" t="s">
-        <v>216</v>
+      <c r="C47" s="21" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B48" s="20">
+      <c r="B48" s="19">
         <f t="shared" si="1"/>
         <v>3.1599999999999988</v>
       </c>
-      <c r="C48" s="22" t="s">
-        <v>217</v>
+      <c r="C48" s="21" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B49" s="20">
+      <c r="B49" s="19">
         <f t="shared" si="1"/>
         <v>3.1699999999999986</v>
       </c>
-      <c r="C49" s="22" t="s">
-        <v>218</v>
+      <c r="C49" s="21" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="20">
+      <c r="B50" s="19">
         <f t="shared" si="1"/>
         <v>3.1799999999999984</v>
       </c>
-      <c r="C50" s="22" t="s">
-        <v>219</v>
+      <c r="C50" s="21" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B51" s="20">
+      <c r="B51" s="19">
         <f t="shared" si="1"/>
         <v>3.1899999999999982</v>
       </c>
-      <c r="C51" s="22" t="s">
-        <v>220</v>
+      <c r="C51" s="21" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B52" s="20">
+      <c r="B52" s="19">
         <f t="shared" si="1"/>
         <v>3.199999999999998</v>
       </c>
-      <c r="C52" s="22" t="s">
-        <v>221</v>
+      <c r="C52" s="21" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B53" s="20">
+      <c r="B53" s="19">
         <f t="shared" si="1"/>
         <v>3.2099999999999977</v>
       </c>
-      <c r="C53" s="22" t="s">
-        <v>222</v>
+      <c r="C53" s="21" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A54" s="23" t="s">
-        <v>162</v>
+      <c r="A54" s="22" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C55" s="22" t="s">
+      <c r="C55" s="21" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4693,8 +4682,8 @@
         <f>B55+0.1</f>
         <v>4.1999999999999993</v>
       </c>
-      <c r="C56" s="22" t="s">
-        <v>223</v>
+      <c r="C56" s="21" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4702,8 +4691,8 @@
         <f t="shared" ref="B57:B63" si="2">B56+0.1</f>
         <v>4.2999999999999989</v>
       </c>
-      <c r="C57" s="22" t="s">
-        <v>224</v>
+      <c r="C57" s="21" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4711,8 +4700,8 @@
         <f t="shared" si="2"/>
         <v>4.3999999999999986</v>
       </c>
-      <c r="C58" s="22" t="s">
-        <v>225</v>
+      <c r="C58" s="21" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4720,8 +4709,8 @@
         <f t="shared" si="2"/>
         <v>4.4999999999999982</v>
       </c>
-      <c r="C59" s="22" t="s">
-        <v>226</v>
+      <c r="C59" s="21" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4729,8 +4718,8 @@
         <f t="shared" si="2"/>
         <v>4.5999999999999979</v>
       </c>
-      <c r="C60" s="22" t="s">
-        <v>227</v>
+      <c r="C60" s="21" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4738,8 +4727,8 @@
         <f t="shared" si="2"/>
         <v>4.6999999999999975</v>
       </c>
-      <c r="C61" s="22" t="s">
-        <v>228</v>
+      <c r="C61" s="21" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4747,8 +4736,8 @@
         <f t="shared" si="2"/>
         <v>4.7999999999999972</v>
       </c>
-      <c r="C62" s="22" t="s">
-        <v>229</v>
+      <c r="C62" s="21" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4756,16 +4745,16 @@
         <f t="shared" si="2"/>
         <v>4.8999999999999968</v>
       </c>
-      <c r="C63" s="22" t="s">
+      <c r="C63" s="21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B64" s="19">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C64" s="21" t="s">
         <v>230</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B64" s="20">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C64" s="22" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4773,8 +4762,8 @@
         <f t="shared" ref="B65:B73" si="3">B64+0.01</f>
         <v>4.1099999999999994</v>
       </c>
-      <c r="C65" s="22" t="s">
-        <v>232</v>
+      <c r="C65" s="21" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4782,8 +4771,8 @@
         <f t="shared" si="3"/>
         <v>4.1199999999999992</v>
       </c>
-      <c r="C66" s="22" t="s">
-        <v>233</v>
+      <c r="C66" s="21" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4791,8 +4780,8 @@
         <f t="shared" si="3"/>
         <v>4.129999999999999</v>
       </c>
-      <c r="C67" s="22" t="s">
-        <v>234</v>
+      <c r="C67" s="21" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4800,8 +4789,8 @@
         <f t="shared" si="3"/>
         <v>4.1399999999999988</v>
       </c>
-      <c r="C68" s="22" t="s">
-        <v>235</v>
+      <c r="C68" s="21" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4809,8 +4798,8 @@
         <f t="shared" si="3"/>
         <v>4.1499999999999986</v>
       </c>
-      <c r="C69" s="22" t="s">
-        <v>236</v>
+      <c r="C69" s="21" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4818,8 +4807,8 @@
         <f t="shared" si="3"/>
         <v>4.1599999999999984</v>
       </c>
-      <c r="C70" s="22" t="s">
-        <v>237</v>
+      <c r="C70" s="21" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4827,8 +4816,8 @@
         <f t="shared" si="3"/>
         <v>4.1699999999999982</v>
       </c>
-      <c r="C71" s="22" t="s">
-        <v>238</v>
+      <c r="C71" s="21" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4836,8 +4825,8 @@
         <f t="shared" si="3"/>
         <v>4.1799999999999979</v>
       </c>
-      <c r="C72" s="22" t="s">
-        <v>239</v>
+      <c r="C72" s="21" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4845,24 +4834,24 @@
         <f t="shared" si="3"/>
         <v>4.1899999999999977</v>
       </c>
-      <c r="C73" s="22" t="s">
-        <v>240</v>
+      <c r="C73" s="21" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C74" s="16"/>
+      <c r="C74" s="15"/>
     </row>
     <row r="75" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="23" t="s">
-        <v>163</v>
+      <c r="A75" s="22" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C76" s="22" t="s">
-        <v>241</v>
+      <c r="C76" s="21" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4870,8 +4859,8 @@
         <f>B76+0.1</f>
         <v>5.1999999999999993</v>
       </c>
-      <c r="C77" s="22" t="s">
-        <v>242</v>
+      <c r="C77" s="21" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4879,8 +4868,8 @@
         <f t="shared" ref="B78:B84" si="4">B77+0.1</f>
         <v>5.2999999999999989</v>
       </c>
-      <c r="C78" s="22" t="s">
-        <v>243</v>
+      <c r="C78" s="21" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4888,8 +4877,8 @@
         <f t="shared" si="4"/>
         <v>5.3999999999999986</v>
       </c>
-      <c r="C79" s="22" t="s">
-        <v>244</v>
+      <c r="C79" s="21" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4897,8 +4886,8 @@
         <f t="shared" si="4"/>
         <v>5.4999999999999982</v>
       </c>
-      <c r="C80" s="22" t="s">
-        <v>245</v>
+      <c r="C80" s="21" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4906,8 +4895,8 @@
         <f t="shared" si="4"/>
         <v>5.5999999999999979</v>
       </c>
-      <c r="C81" s="22" t="s">
-        <v>246</v>
+      <c r="C81" s="21" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4915,8 +4904,8 @@
         <f t="shared" si="4"/>
         <v>5.6999999999999975</v>
       </c>
-      <c r="C82" s="22" t="s">
-        <v>247</v>
+      <c r="C82" s="21" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4924,8 +4913,8 @@
         <f t="shared" si="4"/>
         <v>5.7999999999999972</v>
       </c>
-      <c r="C83" s="22" t="s">
-        <v>248</v>
+      <c r="C83" s="21" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4933,16 +4922,16 @@
         <f t="shared" si="4"/>
         <v>5.8999999999999968</v>
       </c>
-      <c r="C84" s="22" t="s">
+      <c r="C84" s="21" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B85" s="19">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C85" s="21" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B85" s="20">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C85" s="22" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4950,8 +4939,8 @@
         <f t="shared" ref="B86:B87" si="5">B85+0.01</f>
         <v>5.1099999999999994</v>
       </c>
-      <c r="C86" s="22" t="s">
-        <v>251</v>
+      <c r="C86" s="21" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4959,21 +4948,21 @@
         <f t="shared" si="5"/>
         <v>5.1199999999999992</v>
       </c>
-      <c r="C87" s="22" t="s">
-        <v>252</v>
+      <c r="C87" s="21" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A88" s="23" t="s">
-        <v>164</v>
+      <c r="A88" s="22" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>6.1</v>
       </c>
-      <c r="C89" s="22" t="s">
-        <v>253</v>
+      <c r="C89" s="21" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4981,8 +4970,8 @@
         <f>B89+0.1</f>
         <v>6.1999999999999993</v>
       </c>
-      <c r="C90" s="22" t="s">
-        <v>254</v>
+      <c r="C90" s="21" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4990,8 +4979,8 @@
         <f t="shared" ref="B91:B97" si="6">B90+0.1</f>
         <v>6.2999999999999989</v>
       </c>
-      <c r="C91" s="22" t="s">
-        <v>255</v>
+      <c r="C91" s="21" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4999,8 +4988,8 @@
         <f t="shared" si="6"/>
         <v>6.3999999999999986</v>
       </c>
-      <c r="C92" s="22" t="s">
-        <v>256</v>
+      <c r="C92" s="21" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -5008,8 +4997,8 @@
         <f t="shared" si="6"/>
         <v>6.4999999999999982</v>
       </c>
-      <c r="C93" s="22" t="s">
-        <v>257</v>
+      <c r="C93" s="21" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -5017,8 +5006,8 @@
         <f t="shared" si="6"/>
         <v>6.5999999999999979</v>
       </c>
-      <c r="C94" s="22" t="s">
-        <v>258</v>
+      <c r="C94" s="21" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -5026,8 +5015,8 @@
         <f t="shared" si="6"/>
         <v>6.6999999999999975</v>
       </c>
-      <c r="C95" s="22" t="s">
-        <v>259</v>
+      <c r="C95" s="21" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -5035,8 +5024,8 @@
         <f t="shared" si="6"/>
         <v>6.7999999999999972</v>
       </c>
-      <c r="C96" s="22" t="s">
-        <v>260</v>
+      <c r="C96" s="21" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="97" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -5044,205 +5033,205 @@
         <f t="shared" si="6"/>
         <v>6.8999999999999968</v>
       </c>
-      <c r="C97" s="22" t="s">
-        <v>261</v>
+      <c r="C97" s="21" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="20"/>
-      <c r="C98" s="15"/>
+      <c r="B98" s="19"/>
+      <c r="C98" s="14"/>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C99" s="17"/>
+      <c r="C99" s="16"/>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C100" s="17"/>
+      <c r="C100" s="16"/>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C101" s="17"/>
+      <c r="C101" s="16"/>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C102" s="17"/>
+      <c r="C102" s="16"/>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C103" s="17"/>
+      <c r="C103" s="16"/>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C104" s="17"/>
+      <c r="C104" s="16"/>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C105" s="18"/>
+      <c r="C105" s="17"/>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C106" s="17"/>
+      <c r="C106" s="16"/>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C107" s="17"/>
+      <c r="C107" s="16"/>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C108" s="18"/>
+      <c r="C108" s="17"/>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C109" s="17"/>
+      <c r="C109" s="16"/>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C110" s="18"/>
+      <c r="C110" s="17"/>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C111" s="17"/>
+      <c r="C111" s="16"/>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C112" s="17"/>
+      <c r="C112" s="16"/>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C113" s="17"/>
+      <c r="C113" s="16"/>
     </row>
     <row r="114" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C114" s="17"/>
+      <c r="C114" s="16"/>
     </row>
     <row r="115" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C115" s="18"/>
+      <c r="C115" s="17"/>
     </row>
     <row r="116" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C116" s="17"/>
+      <c r="C116" s="16"/>
     </row>
     <row r="117" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C117" s="17"/>
+      <c r="C117" s="16"/>
     </row>
     <row r="118" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C118" s="18"/>
+      <c r="C118" s="17"/>
     </row>
     <row r="120" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C120" s="17"/>
+      <c r="C120" s="16"/>
     </row>
     <row r="121" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C121" s="17" t="s">
+      <c r="C121" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C122" s="16" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C122" s="17" t="s">
+    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C123" s="16" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C123" s="17" t="s">
+    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C124" s="16" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C124" s="17" t="s">
+    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C125" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C126" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C127" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C128" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C129" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C130" s="16" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C125" s="17" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C126" s="17" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C127" s="17" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C128" s="17" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C129" s="17" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C130" s="17" t="s">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C131" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C132" s="18" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C131" s="17" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C132" s="19" t="s">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C133" s="16" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C133" s="17" t="s">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C134" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C135" s="16" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C134" s="17" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C135" s="17" t="s">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C136" s="16" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C136" s="17" t="s">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C137" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C138" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C139" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C140" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C141" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C142" s="16" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C137" s="17" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C138" s="17" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C139" s="17" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C140" s="17" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C141" s="17" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C142" s="17" t="s">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C143" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C144" s="16" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C143" s="17" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C144" s="17" t="s">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C145" s="16" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C145" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
     <row r="146" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C146" s="17" t="s">
-        <v>175</v>
+      <c r="C146" s="16" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios script en indicador de prueba
</commit_message>
<xml_diff>
--- a/Listado Indicadores/Listado de indicadores a trabajar.xlsx
+++ b/Listado Indicadores/Listado de indicadores a trabajar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inegobgt-my.sharepoint.com/personal/unidadgenero_ine_gob_gt/Documents/Documentos/Githob/CompendioGenero2023/Listado Indicadores/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inegobgt-my.sharepoint.com/personal/pgalvez_ine_gob_gt/Documents/Documentos/GitHub/CompendioGenero2023/Listado Indicadores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="632" documentId="8_{33C4EBF3-B6E3-430A-80A9-911051E32003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02CC688A-4EDE-4A8D-A9CF-5AEDFCB92521}"/>
+  <xr:revisionPtr revIDLastSave="645" documentId="8_{33C4EBF3-B6E3-430A-80A9-911051E32003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{414CE03F-E6C6-483F-B7E2-816131A3591C}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="17325" windowHeight="15585" xr2:uid="{3D4A4D73-1AC6-4F09-9897-696579B6A714}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3D4A4D73-1AC6-4F09-9897-696579B6A714}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2094,7 +2094,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2188,13 +2188,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2326,7 +2319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2379,9 +2372,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2393,15 +2383,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2410,11 +2396,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2736,10 +2725,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1F1446-4590-4473-8B94-EB49B6294D9F}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2751,1001 +2741,1001 @@
     <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="27" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25" t="s">
+      <c r="C4" s="24"/>
+      <c r="D4" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25" t="s">
+      <c r="C5" s="24"/>
+      <c r="D5" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>233</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25" t="s">
+      <c r="C7" s="24"/>
+      <c r="D7" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25" t="s">
+      <c r="C8" s="24"/>
+      <c r="D8" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25" t="s">
+      <c r="C9" s="24"/>
+      <c r="D9" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25" t="s">
+      <c r="C10" s="24"/>
+      <c r="D10" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25" t="s">
+      <c r="F10" s="24"/>
+      <c r="G10" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25" t="s">
+      <c r="C11" s="24"/>
+      <c r="D11" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25" t="s">
+      <c r="F11" s="24"/>
+      <c r="G11" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25" t="s">
+      <c r="C12" s="24"/>
+      <c r="D12" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25" t="s">
+      <c r="F12" s="24"/>
+      <c r="G12" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
         <v>238</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25" t="s">
+      <c r="C13" s="24"/>
+      <c r="D13" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25" t="s">
+      <c r="F13" s="24"/>
+      <c r="G13" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25" t="s">
+      <c r="C14" s="24"/>
+      <c r="D14" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25" t="s">
+      <c r="F14" s="24"/>
+      <c r="G14" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25" t="s">
+      <c r="C15" s="24"/>
+      <c r="D15" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25" t="s">
+      <c r="C16" s="24"/>
+      <c r="D16" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25" t="s">
+      <c r="F16" s="24"/>
+      <c r="G16" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25" t="s">
+      <c r="C17" s="24"/>
+      <c r="D17" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25" t="s">
+      <c r="F17" s="24"/>
+      <c r="G17" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25" t="s">
+      <c r="C18" s="24"/>
+      <c r="D18" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25" t="s">
+      <c r="F18" s="24"/>
+      <c r="G18" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
         <v>248</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27" t="s">
+      <c r="C19" s="25"/>
+      <c r="D19" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="36" t="s">
+      <c r="F19" s="25"/>
+      <c r="G19" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27" t="s">
+      <c r="C20" s="25"/>
+      <c r="D20" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="36" t="s">
+      <c r="F20" s="25"/>
+      <c r="G20" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
         <v>240</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27" t="s">
+      <c r="C21" s="25"/>
+      <c r="D21" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
+      <c r="F21" s="25"/>
+      <c r="G21" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27" t="s">
+      <c r="C22" s="25"/>
+      <c r="D22" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
+      <c r="F22" s="25"/>
+      <c r="G22" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
         <v>249</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27" t="s">
+      <c r="C23" s="25"/>
+      <c r="D23" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
+      <c r="F23" s="25"/>
+      <c r="G23" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27" t="s">
+      <c r="C24" s="25"/>
+      <c r="D24" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
+      <c r="F24" s="25"/>
+      <c r="G24" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27" t="s">
+      <c r="C25" s="25"/>
+      <c r="D25" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="27" t="s">
+      <c r="E25" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
+      <c r="F25" s="25"/>
+      <c r="G25" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
         <v>241</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27" t="s">
+      <c r="C26" s="25"/>
+      <c r="D26" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
+      <c r="F26" s="25"/>
+      <c r="G26" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
         <v>250</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27" t="s">
+      <c r="C27" s="25"/>
+      <c r="D27" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
+      <c r="F27" s="25"/>
+      <c r="G27" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
         <v>251</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27" t="s">
+      <c r="C28" s="25"/>
+      <c r="D28" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="27" t="s">
+      <c r="F28" s="25" t="s">
         <v>231</v>
       </c>
-      <c r="G28" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
+      <c r="G28" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27" t="s">
+      <c r="C29" s="25"/>
+      <c r="D29" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="E29" s="27" t="s">
+      <c r="E29" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F29" s="27" t="s">
+      <c r="F29" s="25" t="s">
         <v>231</v>
       </c>
-      <c r="G29" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
+      <c r="G29" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27" t="s">
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
+      <c r="F30" s="25"/>
+      <c r="G30" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
         <v>242</v>
       </c>
-      <c r="B31" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31" t="s">
+      <c r="B31" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F31" s="31" t="s">
+      <c r="E31" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="G31" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
+      <c r="G31" s="28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E32" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F32" s="31" t="s">
+      <c r="B32" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="G32" s="31" t="s">
+      <c r="G32" s="28" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="32" t="s">
         <v>243</v>
       </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-    </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="32" t="s">
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+    </row>
+    <row r="34" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="29" t="s">
         <v>244</v>
       </c>
-      <c r="B34" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E34" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31" t="s">
+      <c r="B34" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
+    <row r="35" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E35" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31" t="s">
+      <c r="B35" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E36" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31" t="s">
+      <c r="B36" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="32" t="s">
+    <row r="37" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E37" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31" t="s">
+      <c r="B37" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="32" t="s">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E38" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31" t="s">
+      <c r="B38" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="33" t="s">
+    <row r="39" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="E39" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34" t="s">
+      <c r="B39" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="32" t="s">
+    <row r="40" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="29" t="s">
         <v>245</v>
       </c>
-      <c r="B40" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E40" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="35" t="s">
+      <c r="B40" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="B41" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E41" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="35" t="s">
+      <c r="B41" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="B42" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E42" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="35" t="s">
+      <c r="B42" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="32" t="s">
         <v>253</v>
       </c>
-      <c r="B43" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E43" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="35" t="s">
+      <c r="B43" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F43" s="28"/>
+      <c r="G43" s="28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="32" t="s">
         <v>254</v>
       </c>
-      <c r="B44" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E44" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="35" t="s">
+      <c r="B44" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="32" t="s">
         <v>184</v>
       </c>
-      <c r="B45" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E45" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="35" t="s">
+      <c r="B45" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E45" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="B46" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E46" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="35" t="s">
+      <c r="B46" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F46" s="28"/>
+      <c r="G46" s="28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="B47" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E47" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="35" t="s">
+      <c r="B47" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="28"/>
+      <c r="G47" s="28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="B48" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E48" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="35" t="s">
+      <c r="B48" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E48" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F48" s="28"/>
+      <c r="G48" s="28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="32" t="s">
         <v>188</v>
       </c>
-      <c r="B49" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E49" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F49" s="31" t="s">
+      <c r="B49" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F49" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="G49" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="35" t="s">
+      <c r="G49" s="28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="32" t="s">
         <v>255</v>
       </c>
-      <c r="B50" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E50" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F50" s="31" t="s">
+      <c r="B50" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E50" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F50" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="G50" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="35" t="s">
+      <c r="G50" s="28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="B51" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31" t="s">
+      <c r="B51" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="E51" s="31" t="s">
+      <c r="E51" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F51" s="31"/>
-      <c r="G51" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="22" t="s">
+      <c r="F51" s="28"/>
+      <c r="G51" s="28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B52" t="s">
@@ -3761,7 +3751,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>43</v>
       </c>
@@ -3778,7 +3768,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>44</v>
       </c>
@@ -3798,7 +3788,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>9</v>
       </c>
@@ -3815,7 +3805,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>10</v>
       </c>
@@ -3832,7 +3822,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>11</v>
       </c>
@@ -3852,7 +3842,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>46</v>
       </c>
@@ -3869,7 +3859,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>12</v>
       </c>
@@ -3889,7 +3879,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>47</v>
       </c>
@@ -3909,7 +3899,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>13</v>
       </c>
@@ -3929,7 +3919,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>14</v>
       </c>
@@ -3946,7 +3936,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>15</v>
       </c>
@@ -3966,7 +3956,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>16</v>
       </c>
@@ -3983,7 +3973,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>48</v>
       </c>
@@ -4003,7 +3993,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>17</v>
       </c>
@@ -4023,7 +4013,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>18</v>
       </c>
@@ -4040,7 +4030,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>19</v>
       </c>
@@ -4060,7 +4050,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -4077,7 +4067,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>21</v>
       </c>
@@ -4097,7 +4087,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>22</v>
       </c>
@@ -4120,7 +4110,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>106</v>
       </c>
@@ -4137,7 +4127,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>107</v>
       </c>
@@ -4154,7 +4144,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>68</v>
       </c>
@@ -4171,7 +4161,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>23</v>
       </c>
@@ -4191,7 +4181,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>24</v>
       </c>
@@ -4208,7 +4198,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>69</v>
       </c>
@@ -4225,7 +4215,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>70</v>
       </c>
@@ -4245,7 +4235,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>71</v>
       </c>
@@ -4265,7 +4255,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>111</v>
       </c>
@@ -4282,7 +4272,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>25</v>
       </c>
@@ -4299,7 +4289,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>114</v>
       </c>
@@ -4316,7 +4306,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>26</v>
       </c>
@@ -4333,7 +4323,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>27</v>
       </c>
@@ -4350,7 +4340,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -4367,7 +4357,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>29</v>
       </c>
@@ -4384,7 +4374,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>30</v>
       </c>
@@ -4401,7 +4391,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>31</v>
       </c>
@@ -4418,7 +4408,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>32</v>
       </c>
@@ -4435,7 +4425,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>49</v>
       </c>
@@ -4455,8 +4445,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="21" t="s">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="20" t="s">
         <v>65</v>
       </c>
       <c r="D91" t="s">
@@ -4472,8 +4462,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="21" t="s">
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="20" t="s">
         <v>66</v>
       </c>
       <c r="D92" t="s">
@@ -4486,8 +4476,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="21" t="s">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="20" t="s">
         <v>72</v>
       </c>
       <c r="B93" t="s">
@@ -4506,8 +4496,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="21" t="s">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="20" t="s">
         <v>73</v>
       </c>
       <c r="D94" t="s">
@@ -4523,8 +4513,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="21" t="s">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="20" t="s">
         <v>77</v>
       </c>
       <c r="D95" t="s">
@@ -4540,8 +4530,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="21" t="s">
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="20" t="s">
         <v>78</v>
       </c>
       <c r="D96" t="s">
@@ -4557,8 +4547,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="21" t="s">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="20" t="s">
         <v>80</v>
       </c>
       <c r="D97" t="s">
@@ -4571,8 +4561,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="21" t="s">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="20" t="s">
         <v>83</v>
       </c>
       <c r="C98" s="4"/>
@@ -4586,8 +4576,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="21" t="s">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="20" t="s">
         <v>84</v>
       </c>
       <c r="D99" t="s">
@@ -4600,7 +4590,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>110</v>
       </c>
@@ -4614,7 +4604,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>115</v>
       </c>
@@ -4634,7 +4624,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>118</v>
       </c>
@@ -4651,7 +4641,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>121</v>
       </c>
@@ -4665,7 +4655,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>122</v>
       </c>
@@ -4682,7 +4672,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>124</v>
       </c>
@@ -4699,8 +4689,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="21" t="s">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="20" t="s">
         <v>82</v>
       </c>
       <c r="D106" t="s">
@@ -4714,7 +4704,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G106" xr:uid="{0A1F1446-4590-4473-8B94-EB49B6294D9F}"/>
+  <autoFilter ref="A1:G106" xr:uid="{0A1F1446-4590-4473-8B94-EB49B6294D9F}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="CENSO"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4740,7 +4736,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="18">
         <v>1.1000000000000001</v>
       </c>
@@ -4749,7 +4745,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
+      <c r="A3" s="34"/>
       <c r="B3" s="18">
         <v>1.2</v>
       </c>
@@ -4758,7 +4754,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="18">
         <v>1.3</v>
       </c>
@@ -4767,7 +4763,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="18">
         <v>1.4</v>
       </c>
@@ -4776,7 +4772,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="18">
         <v>1.5</v>
       </c>
@@ -4785,7 +4781,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="18">
         <v>1.6</v>
       </c>
@@ -4794,7 +4790,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="18">
         <v>1.7</v>
       </c>
@@ -4803,7 +4799,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="18">
         <v>1.8</v>
       </c>

</xml_diff>